<commit_message>
error in github link
</commit_message>
<xml_diff>
--- a/indicators/NO_GJEN_001/metadata.xlsx
+++ b/indicators/NO_GJEN_001/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anders.kolstad\Github\ecRxiv\indicators\NO_GJEN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\41001581_egenutvikling_anders_kolstad\github\ecRxiv\indicators\NO_GJEN_001\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A955DE-7A36-4CE4-B563-28FE783F9C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452F4D16-4911-408B-97BA-C67F8068DBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="38700" windowHeight="15375" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="38700" windowHeight="15375" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -573,10 +573,10 @@
     <t>Mienna, I., M., Venter, Z.</t>
   </si>
   <si>
-    <t>https://github.com/NINAnor/ecRxiv/tree/main/indicators/NO_GJEN</t>
-  </si>
-  <si>
     <t>yearAdded</t>
+  </si>
+  <si>
+    <t>https://github.com/NINAnor/ecRxiv/tree/main/indicators/NO_GJEN_001</t>
   </si>
 </sst>
 </file>
@@ -1022,7 +1022,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B14" s="2">
         <v>2024</v>
@@ -1218,7 +1218,7 @@
         <v>172</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>

</xml_diff>